<commit_message>
Done comparision in 2018 November
</commit_message>
<xml_diff>
--- a/probList.xlsx
+++ b/probList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo\Source\eVUl1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F350024E-B2AB-4D0A-B182-5576FE58225A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3818D7AE-D963-47CE-9FAF-76C9BEDBA78C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" xr2:uid="{0251418C-5C45-4AA2-B575-F82157FE28AE}"/>
   </bookViews>
@@ -904,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{956BC141-9A20-49AB-9DF6-AF3A59252D84}">
   <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,46 +986,46 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="B4" s="4">
         <v>4</v>
       </c>
-      <c r="C4" s="5">
-        <v>3089</v>
-      </c>
-      <c r="D4" s="5">
-        <v>4000</v>
-      </c>
+      <c r="C4" s="4">
+        <v>150</v>
+      </c>
+      <c r="D4" s="4"/>
       <c r="E4" s="2" t="s">
-        <v>73</v>
+        <v>8</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="B5" s="4">
         <v>4</v>
       </c>
-      <c r="C5" s="4">
-        <v>150</v>
-      </c>
-      <c r="D5" s="4"/>
+      <c r="C5" s="5">
+        <v>3089</v>
+      </c>
+      <c r="D5" s="5">
+        <v>4000</v>
+      </c>
       <c r="E5" s="2" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1053,17 +1053,17 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B7" s="4">
         <v>6</v>
       </c>
       <c r="C7" s="5">
-        <v>3107</v>
+        <v>1385</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="2" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>127</v>
@@ -1072,17 +1072,17 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B8" s="4">
         <v>6</v>
       </c>
       <c r="C8" s="5">
-        <v>1385</v>
+        <v>3107</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="2" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>127</v>
@@ -1110,24 +1110,22 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>126</v>
       </c>
       <c r="B10" s="4">
         <v>8</v>
       </c>
       <c r="C10" s="5">
-        <v>59535</v>
+        <v>4177</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="4">
-        <v>2</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -1150,22 +1148,24 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>126</v>
+        <v>23</v>
       </c>
       <c r="B12" s="4">
         <v>8</v>
       </c>
       <c r="C12" s="5">
-        <v>4177</v>
+        <v>59535</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="2" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="G12" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="G12" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -1190,61 +1190,59 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="B14" s="4">
         <v>9</v>
       </c>
-      <c r="C14" s="5">
-        <v>43500</v>
-      </c>
-      <c r="D14" s="5">
-        <v>14500</v>
-      </c>
+      <c r="C14" s="4">
+        <v>214</v>
+      </c>
+      <c r="D14" s="4"/>
       <c r="E14" s="2" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G14" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="B15" s="4">
         <v>9</v>
       </c>
-      <c r="C15" s="4">
-        <v>214</v>
-      </c>
-      <c r="D15" s="4"/>
+      <c r="C15" s="5">
+        <v>43500</v>
+      </c>
+      <c r="D15" s="5">
+        <v>14500</v>
+      </c>
       <c r="E15" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="B16" s="4">
         <v>10</v>
       </c>
-      <c r="C16" s="5">
-        <v>25010</v>
-      </c>
-      <c r="D16" s="5">
-        <v>1000000</v>
-      </c>
+      <c r="C16" s="4">
+        <v>683</v>
+      </c>
+      <c r="D16" s="4"/>
       <c r="E16" s="2" t="s">
         <v>8</v>
       </c>
@@ -1252,20 +1250,22 @@
         <v>9</v>
       </c>
       <c r="G16" s="4">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="B17" s="4">
         <v>10</v>
       </c>
-      <c r="C17" s="4">
-        <v>683</v>
-      </c>
-      <c r="D17" s="4"/>
+      <c r="C17" s="5">
+        <v>25010</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1000000</v>
+      </c>
       <c r="E17" s="2" t="s">
         <v>8</v>
       </c>
@@ -1273,53 +1273,53 @@
         <v>9</v>
       </c>
       <c r="G17" s="4">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B18" s="4">
         <v>10</v>
       </c>
       <c r="C18" s="4">
-        <v>528</v>
+        <v>300</v>
       </c>
       <c r="D18" s="4">
-        <v>462</v>
+        <v>312</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G18" s="4">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B19" s="4">
         <v>10</v>
       </c>
       <c r="C19" s="4">
-        <v>300</v>
+        <v>528</v>
       </c>
       <c r="D19" s="4">
-        <v>312</v>
+        <v>462</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>73</v>
+        <v>8</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="4">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1343,43 +1343,43 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>136</v>
+        <v>42</v>
       </c>
       <c r="B21" s="4">
         <v>13</v>
       </c>
       <c r="C21" s="4">
-        <v>506</v>
+        <v>270</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="G21" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="G21" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>42</v>
+        <v>136</v>
       </c>
       <c r="B22" s="4">
         <v>13</v>
       </c>
       <c r="C22" s="4">
-        <v>270</v>
+        <v>506</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="2" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="4">
-        <v>2</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
@@ -1444,68 +1444,68 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>95</v>
+        <v>135</v>
       </c>
       <c r="B26" s="4">
         <v>16</v>
       </c>
-      <c r="C26" s="5">
-        <v>15000</v>
-      </c>
-      <c r="D26" s="5">
-        <v>5000</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="C26" s="4">
+        <v>336</v>
+      </c>
+      <c r="D26" s="4">
+        <v>31</v>
+      </c>
+      <c r="E26" s="3"/>
       <c r="F26" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G26" s="4">
-        <v>26</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B27" s="4">
         <v>16</v>
       </c>
       <c r="C27" s="5">
-        <v>7494</v>
+        <v>15000</v>
       </c>
       <c r="D27" s="5">
-        <v>3498</v>
+        <v>5000</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G27" s="4">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>135</v>
+        <v>102</v>
       </c>
       <c r="B28" s="4">
         <v>16</v>
       </c>
-      <c r="C28" s="4">
-        <v>336</v>
-      </c>
-      <c r="D28" s="4">
-        <v>31</v>
-      </c>
-      <c r="E28" s="3"/>
+      <c r="C28" s="5">
+        <v>7494</v>
+      </c>
+      <c r="D28" s="5">
+        <v>3498</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F28" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="G28" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="G28" s="4">
+        <v>10</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
@@ -1811,7 +1811,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>27</v>
+        <v>91</v>
       </c>
       <c r="B43" s="4">
         <v>54</v>
@@ -1827,12 +1827,12 @@
         <v>9</v>
       </c>
       <c r="G43" s="4">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>91</v>
+        <v>27</v>
       </c>
       <c r="B44" s="4">
         <v>54</v>
@@ -1848,24 +1848,22 @@
         <v>9</v>
       </c>
       <c r="G44" s="4">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B45" s="4">
         <v>60</v>
       </c>
-      <c r="C45" s="5">
-        <v>1000</v>
-      </c>
-      <c r="D45" s="5">
-        <v>2175</v>
-      </c>
+      <c r="C45" s="4">
+        <v>208</v>
+      </c>
+      <c r="D45" s="4"/>
       <c r="E45" s="2" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>9</v>
@@ -1876,17 +1874,19 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B46" s="4">
         <v>60</v>
       </c>
-      <c r="C46" s="4">
-        <v>208</v>
-      </c>
-      <c r="D46" s="4"/>
+      <c r="C46" s="5">
+        <v>1000</v>
+      </c>
+      <c r="D46" s="5">
+        <v>2175</v>
+      </c>
       <c r="E46" s="2" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>9</v>
@@ -2048,16 +2048,16 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B54" s="4">
         <v>123</v>
       </c>
       <c r="C54" s="5">
-        <v>32561</v>
+        <v>1605</v>
       </c>
       <c r="D54" s="5">
-        <v>16281</v>
+        <v>30956</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>8</v>
@@ -2071,16 +2071,16 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B55" s="4">
         <v>123</v>
       </c>
       <c r="C55" s="5">
-        <v>22696</v>
+        <v>2265</v>
       </c>
       <c r="D55" s="5">
-        <v>9865</v>
+        <v>30296</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>8</v>
@@ -2094,16 +2094,16 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B56" s="4">
         <v>123</v>
       </c>
       <c r="C56" s="5">
-        <v>16100</v>
+        <v>3185</v>
       </c>
       <c r="D56" s="5">
-        <v>16461</v>
+        <v>29376</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>8</v>
@@ -2117,16 +2117,16 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B57" s="4">
         <v>123</v>
       </c>
       <c r="C57" s="5">
-        <v>11220</v>
+        <v>4781</v>
       </c>
       <c r="D57" s="5">
-        <v>21341</v>
+        <v>27780</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>8</v>
@@ -2163,16 +2163,16 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B59" s="4">
         <v>123</v>
       </c>
       <c r="C59" s="5">
-        <v>4781</v>
+        <v>11220</v>
       </c>
       <c r="D59" s="5">
-        <v>27780</v>
+        <v>21341</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>8</v>
@@ -2186,16 +2186,16 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B60" s="4">
         <v>123</v>
       </c>
       <c r="C60" s="5">
-        <v>3185</v>
+        <v>16100</v>
       </c>
       <c r="D60" s="5">
-        <v>29376</v>
+        <v>16461</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>8</v>
@@ -2209,16 +2209,16 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B61" s="4">
         <v>123</v>
       </c>
       <c r="C61" s="5">
-        <v>2265</v>
+        <v>22696</v>
       </c>
       <c r="D61" s="5">
-        <v>30296</v>
+        <v>9865</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>8</v>
@@ -2232,16 +2232,16 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B62" s="4">
         <v>123</v>
       </c>
       <c r="C62" s="5">
-        <v>1605</v>
+        <v>32561</v>
       </c>
       <c r="D62" s="5">
-        <v>30956</v>
+        <v>16281</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>8</v>
@@ -2366,16 +2366,16 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B68" s="4">
         <v>300</v>
       </c>
       <c r="C68" s="5">
-        <v>49749</v>
+        <v>2477</v>
       </c>
       <c r="D68" s="5">
-        <v>14951</v>
+        <v>47272</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>78</v>
@@ -2389,16 +2389,16 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B69" s="4">
         <v>300</v>
       </c>
       <c r="C69" s="5">
-        <v>24692</v>
+        <v>3470</v>
       </c>
       <c r="D69" s="5">
-        <v>25057</v>
+        <v>46279</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>78</v>
@@ -2412,16 +2412,16 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B70" s="4">
         <v>300</v>
       </c>
       <c r="C70" s="5">
-        <v>17188</v>
+        <v>4912</v>
       </c>
       <c r="D70" s="5">
-        <v>32561</v>
+        <v>44837</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>78</v>
@@ -2435,16 +2435,16 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B71" s="4">
         <v>300</v>
       </c>
       <c r="C71" s="5">
-        <v>9888</v>
+        <v>7366</v>
       </c>
       <c r="D71" s="5">
-        <v>39861</v>
+        <v>42383</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>78</v>
@@ -2458,16 +2458,16 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B72" s="4">
         <v>300</v>
       </c>
       <c r="C72" s="5">
-        <v>7366</v>
+        <v>9888</v>
       </c>
       <c r="D72" s="5">
-        <v>42383</v>
+        <v>39861</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>78</v>
@@ -2481,16 +2481,16 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B73" s="4">
         <v>300</v>
       </c>
       <c r="C73" s="5">
-        <v>4912</v>
+        <v>17188</v>
       </c>
       <c r="D73" s="5">
-        <v>44837</v>
+        <v>32561</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>78</v>
@@ -2504,16 +2504,16 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B74" s="4">
         <v>300</v>
       </c>
       <c r="C74" s="5">
-        <v>3470</v>
+        <v>24692</v>
       </c>
       <c r="D74" s="5">
-        <v>46279</v>
+        <v>25057</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>78</v>
@@ -2527,16 +2527,16 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B75" s="4">
         <v>300</v>
       </c>
       <c r="C75" s="5">
-        <v>2477</v>
+        <v>49749</v>
       </c>
       <c r="D75" s="5">
-        <v>47272</v>
+        <v>14951</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>78</v>
@@ -2638,21 +2638,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B80" s="5">
         <v>2000</v>
       </c>
-      <c r="C80" s="5">
-        <v>400000</v>
-      </c>
-      <c r="D80" s="5">
-        <v>100000</v>
-      </c>
+      <c r="C80" s="4">
+        <v>62</v>
+      </c>
+      <c r="D80" s="4"/>
       <c r="E80" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="F80" s="3" t="s">
         <v>9</v>
@@ -2661,19 +2659,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B81" s="5">
         <v>2000</v>
       </c>
-      <c r="C81" s="4">
-        <v>62</v>
-      </c>
-      <c r="D81" s="4"/>
+      <c r="C81" s="5">
+        <v>400000</v>
+      </c>
+      <c r="D81" s="5">
+        <v>100000</v>
+      </c>
       <c r="E81" s="2" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="F81" s="3" t="s">
         <v>9</v>
@@ -2816,55 +2816,55 @@
         <v>22</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>148</v>
+        <v>61</v>
       </c>
       <c r="B88" s="5">
         <v>47236</v>
       </c>
       <c r="C88" s="5">
-        <v>23149</v>
+        <v>20242</v>
       </c>
       <c r="D88" s="5">
-        <v>781265</v>
+        <v>677399</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>62</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>146</v>
+        <v>9</v>
       </c>
       <c r="G88" s="4">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>149</v>
+        <v>106</v>
       </c>
       <c r="B89" s="5">
         <v>47236</v>
       </c>
       <c r="C89" s="5">
-        <v>23149</v>
+        <v>15564</v>
       </c>
       <c r="D89" s="5">
-        <v>781265</v>
+        <v>518571</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>62</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>146</v>
+        <v>9</v>
       </c>
       <c r="G89" s="4">
-        <v>313</v>
+        <v>53</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B90" s="5">
         <v>47236</v>
@@ -2882,53 +2882,53 @@
         <v>146</v>
       </c>
       <c r="G90" s="4">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>61</v>
+        <v>150</v>
       </c>
       <c r="B91" s="5">
         <v>47236</v>
       </c>
       <c r="C91" s="5">
-        <v>20242</v>
+        <v>23149</v>
       </c>
       <c r="D91" s="5">
-        <v>677399</v>
+        <v>781265</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>62</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>9</v>
+        <v>146</v>
       </c>
       <c r="G91" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>106</v>
+        <v>148</v>
       </c>
       <c r="B92" s="5">
         <v>47236</v>
       </c>
       <c r="C92" s="5">
-        <v>15564</v>
+        <v>23149</v>
       </c>
       <c r="D92" s="5">
-        <v>518571</v>
+        <v>781265</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>62</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>9</v>
+        <v>146</v>
       </c>
       <c r="G92" s="4">
-        <v>53</v>
+        <v>101</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3021,21 +3021,21 @@
       </c>
       <c r="G96" s="4"/>
     </row>
-    <row r="97" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B97" s="5">
         <v>1000000</v>
       </c>
       <c r="C97" s="5">
-        <v>4195197692</v>
+        <v>40428967</v>
       </c>
       <c r="D97" s="5">
-        <v>178274637</v>
+        <v>4577464</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F97" s="3" t="s">
         <v>9</v>
@@ -3067,21 +3067,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B99" s="5">
         <v>1000000</v>
       </c>
       <c r="C99" s="5">
-        <v>40428967</v>
+        <v>4195197692</v>
       </c>
       <c r="D99" s="5">
-        <v>4577464</v>
+        <v>178274637</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F99" s="3" t="s">
         <v>9</v>
@@ -3310,56 +3310,56 @@
     </row>
   </sheetData>
   <sortState ref="A2:G109">
-    <sortCondition ref="B25"/>
+    <sortCondition ref="B1"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="A62" r:id="rId1" location="a1a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - a1a" xr:uid="{AF516471-0A53-43CA-920B-A57E1B40EEF5}"/>
-    <hyperlink ref="E62" r:id="rId2" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{AED66A89-190B-4B24-826A-FDDFFE01DC5C}"/>
-    <hyperlink ref="A61" r:id="rId3" location="a2a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - a2a" xr:uid="{167E31E9-BECD-4E18-8920-EC89E728ECB2}"/>
-    <hyperlink ref="E61" r:id="rId4" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{E2D9CE5B-0E8E-441B-93E3-5DEF01BE3F5A}"/>
-    <hyperlink ref="A60" r:id="rId5" location="a3a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - a3a" xr:uid="{466D13A1-7298-4900-8B58-B56D40013D42}"/>
-    <hyperlink ref="E60" r:id="rId6" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{C017C4F9-38AE-4A82-9B7A-F44B9D379871}"/>
-    <hyperlink ref="A59" r:id="rId7" location="a4a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - a4a" xr:uid="{9994639C-7B9F-4C8A-94A1-317FBDC916FD}"/>
-    <hyperlink ref="E59" r:id="rId8" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{0AE74E8D-CBC8-4156-83B9-D485D9D7E7AD}"/>
+    <hyperlink ref="A54" r:id="rId1" location="a1a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - a1a" xr:uid="{AF516471-0A53-43CA-920B-A57E1B40EEF5}"/>
+    <hyperlink ref="E54" r:id="rId2" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{AED66A89-190B-4B24-826A-FDDFFE01DC5C}"/>
+    <hyperlink ref="A55" r:id="rId3" location="a2a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - a2a" xr:uid="{167E31E9-BECD-4E18-8920-EC89E728ECB2}"/>
+    <hyperlink ref="E55" r:id="rId4" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{E2D9CE5B-0E8E-441B-93E3-5DEF01BE3F5A}"/>
+    <hyperlink ref="A56" r:id="rId5" location="a3a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - a3a" xr:uid="{466D13A1-7298-4900-8B58-B56D40013D42}"/>
+    <hyperlink ref="E56" r:id="rId6" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{C017C4F9-38AE-4A82-9B7A-F44B9D379871}"/>
+    <hyperlink ref="A57" r:id="rId7" location="a4a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - a4a" xr:uid="{9994639C-7B9F-4C8A-94A1-317FBDC916FD}"/>
+    <hyperlink ref="E57" r:id="rId8" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{0AE74E8D-CBC8-4156-83B9-D485D9D7E7AD}"/>
     <hyperlink ref="A58" r:id="rId9" location="a5a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - a5a" xr:uid="{23087B98-C69F-4B8C-B73E-15EB68D8A7C1}"/>
     <hyperlink ref="E58" r:id="rId10" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{5874C5AA-BD9D-4C49-A5E5-E532ED47DCA0}"/>
-    <hyperlink ref="A57" r:id="rId11" location="a6a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - a6a" xr:uid="{7FE947B9-2DD6-4BD3-BE33-DBEA202D1298}"/>
-    <hyperlink ref="E57" r:id="rId12" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{3A3D7FA4-D065-4C20-B454-B42A7567B0D2}"/>
-    <hyperlink ref="A56" r:id="rId13" location="a7a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - a7a" xr:uid="{71FB44C4-D269-4F32-8941-9E037FF474D5}"/>
-    <hyperlink ref="E56" r:id="rId14" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{349CC982-DF89-4ED1-87CA-D4EDDE006959}"/>
-    <hyperlink ref="A55" r:id="rId15" location="a8a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - a8a" xr:uid="{675859AF-D6CC-48E2-A2EA-F5BE9795CF0D}"/>
-    <hyperlink ref="E55" r:id="rId16" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{6C181960-BC5F-4C7B-8476-FDD3CE4B1AED}"/>
-    <hyperlink ref="A54" r:id="rId17" location="a9a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - a9a" xr:uid="{26E59EA0-3685-445C-9A4D-D32A7444F9E7}"/>
-    <hyperlink ref="E54" r:id="rId18" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{8BF56EAB-09CD-47D0-AE97-CD4DE7613FCB}"/>
+    <hyperlink ref="A59" r:id="rId11" location="a6a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - a6a" xr:uid="{7FE947B9-2DD6-4BD3-BE33-DBEA202D1298}"/>
+    <hyperlink ref="E59" r:id="rId12" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{3A3D7FA4-D065-4C20-B454-B42A7567B0D2}"/>
+    <hyperlink ref="A60" r:id="rId13" location="a7a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - a7a" xr:uid="{71FB44C4-D269-4F32-8941-9E037FF474D5}"/>
+    <hyperlink ref="E60" r:id="rId14" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{349CC982-DF89-4ED1-87CA-D4EDDE006959}"/>
+    <hyperlink ref="A61" r:id="rId15" location="a8a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - a8a" xr:uid="{675859AF-D6CC-48E2-A2EA-F5BE9795CF0D}"/>
+    <hyperlink ref="E61" r:id="rId16" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{6C181960-BC5F-4C7B-8476-FDD3CE4B1AED}"/>
+    <hyperlink ref="A62" r:id="rId17" location="a9a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - a9a" xr:uid="{26E59EA0-3685-445C-9A4D-D32A7444F9E7}"/>
+    <hyperlink ref="E62" r:id="rId18" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{8BF56EAB-09CD-47D0-AE97-CD4DE7613FCB}"/>
     <hyperlink ref="A24" r:id="rId19" location="australian" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - australian" xr:uid="{65FCA96C-6057-4742-BC91-E909EA582B9B}"/>
     <hyperlink ref="E24" r:id="rId20" display="http://www.liacc.up.pt/ML/old/statlog/datasets.html" xr:uid="{ACED8CCA-B2C1-4BFD-B8F3-E2D9A82105FF}"/>
-    <hyperlink ref="A99" r:id="rId21" location="avazu" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - avazu" xr:uid="{E6822265-3316-4E23-BF25-0203A921FAE7}"/>
-    <hyperlink ref="E99" r:id="rId22" display="https://www.kaggle.com/c/avazu-ctr-prediction/data" xr:uid="{6F4C1BFB-55E4-4FE2-931E-1D514015B619}"/>
-    <hyperlink ref="A17" r:id="rId23" location="breast-cancer" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - breast-cancer" xr:uid="{0028A195-4A33-4B4F-9E79-252AD5E6D8FB}"/>
-    <hyperlink ref="E17" r:id="rId24" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{F6C935DC-32A9-4084-9B2A-57838EB8275D}"/>
-    <hyperlink ref="A10" r:id="rId25" location="cod-rna" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - cod-rna" xr:uid="{47A532F1-96BA-4332-8C86-80356D103B51}"/>
-    <hyperlink ref="E10" r:id="rId26" location="AVU06a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - AVU06a" xr:uid="{4A0E6316-D819-48BA-80F2-B5CB66269171}"/>
-    <hyperlink ref="A81" r:id="rId27" location="colon-cancer" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - colon-cancer" xr:uid="{C10E750B-9D03-456C-AA6F-165427969959}"/>
-    <hyperlink ref="E81" r:id="rId28" location="AU99a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - AU99a" xr:uid="{387B2AD0-79C7-49EB-8037-2BFAFD6907C5}"/>
-    <hyperlink ref="A43" r:id="rId29" location="covtype.binary" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - covtype.binary" xr:uid="{F4E6A408-B760-44AC-AC56-7F980D042279}"/>
-    <hyperlink ref="E43" r:id="rId30" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{142DBF16-3695-4B61-9993-664AAE35F6F2}"/>
+    <hyperlink ref="A97" r:id="rId21" location="avazu" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - avazu" xr:uid="{E6822265-3316-4E23-BF25-0203A921FAE7}"/>
+    <hyperlink ref="E97" r:id="rId22" display="https://www.kaggle.com/c/avazu-ctr-prediction/data" xr:uid="{6F4C1BFB-55E4-4FE2-931E-1D514015B619}"/>
+    <hyperlink ref="A16" r:id="rId23" location="breast-cancer" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - breast-cancer" xr:uid="{0028A195-4A33-4B4F-9E79-252AD5E6D8FB}"/>
+    <hyperlink ref="E16" r:id="rId24" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{F6C935DC-32A9-4084-9B2A-57838EB8275D}"/>
+    <hyperlink ref="A12" r:id="rId25" location="cod-rna" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - cod-rna" xr:uid="{47A532F1-96BA-4332-8C86-80356D103B51}"/>
+    <hyperlink ref="E12" r:id="rId26" location="AVU06a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - AVU06a" xr:uid="{4A0E6316-D819-48BA-80F2-B5CB66269171}"/>
+    <hyperlink ref="A80" r:id="rId27" location="colon-cancer" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - colon-cancer" xr:uid="{C10E750B-9D03-456C-AA6F-165427969959}"/>
+    <hyperlink ref="E80" r:id="rId28" location="AU99a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - AU99a" xr:uid="{387B2AD0-79C7-49EB-8037-2BFAFD6907C5}"/>
+    <hyperlink ref="A44" r:id="rId29" location="covtype.binary" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - covtype.binary" xr:uid="{F4E6A408-B760-44AC-AC56-7F980D042279}"/>
+    <hyperlink ref="E44" r:id="rId30" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{142DBF16-3695-4B61-9993-664AAE35F6F2}"/>
     <hyperlink ref="A98" r:id="rId31" location="criteo" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - criteo" xr:uid="{B7C3B87C-E640-4C43-A277-92E126F290F7}"/>
     <hyperlink ref="E98" r:id="rId32" display="http://labs.criteo.com/2014/02/kaggle-display-advertising-challenge-dataset/" xr:uid="{2A9BAD02-024E-429A-B9AC-0587A9EDF424}"/>
-    <hyperlink ref="A97" r:id="rId33" location="criteo_tb" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - criteo_tb" xr:uid="{37BDCA0A-E00E-4AB3-B88F-AE1AF356BB2E}"/>
-    <hyperlink ref="E97" r:id="rId34" display="http://labs.criteo.com/2013/12/download-terabyte-click-logs/" xr:uid="{E912CCBF-EC16-4FF2-88B6-F89048070B64}"/>
+    <hyperlink ref="A99" r:id="rId33" location="criteo_tb" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - criteo_tb" xr:uid="{37BDCA0A-E00E-4AB3-B88F-AE1AF356BB2E}"/>
+    <hyperlink ref="E99" r:id="rId34" display="http://labs.criteo.com/2013/12/download-terabyte-click-logs/" xr:uid="{E912CCBF-EC16-4FF2-88B6-F89048070B64}"/>
     <hyperlink ref="A13" r:id="rId35" location="diabetes" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - diabetes" xr:uid="{AB67DE0C-AA35-40D5-AEF6-979A92674782}"/>
     <hyperlink ref="E13" r:id="rId36" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{2985CFAE-2EF6-4C40-8A69-BD70ADC377E1}"/>
     <hyperlink ref="A84" r:id="rId37" location="duke%20breast-cancer" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - duke%20breast-cancer" xr:uid="{BD0C255B-988F-4D11-AFBA-0FA0B8E38E0F}"/>
     <hyperlink ref="E84" r:id="rId38" location="MW01a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - MW01a" xr:uid="{539F6D7E-E9FE-47DF-BC09-EEBC05E6AC72}"/>
-    <hyperlink ref="A80" r:id="rId39" location="epsilon" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - epsilon" xr:uid="{EB3F6D2A-BED8-4AEA-8FAD-FA96A12E346D}"/>
-    <hyperlink ref="E80" r:id="rId40" display="http://largescale.ml.tu-berlin.de/instructions/" xr:uid="{9F1A60A5-2A00-477D-A51C-831A04686117}"/>
+    <hyperlink ref="A81" r:id="rId39" location="epsilon" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - epsilon" xr:uid="{EB3F6D2A-BED8-4AEA-8FAD-FA96A12E346D}"/>
+    <hyperlink ref="E81" r:id="rId40" display="http://largescale.ml.tu-berlin.de/instructions/" xr:uid="{9F1A60A5-2A00-477D-A51C-831A04686117}"/>
     <hyperlink ref="A2" r:id="rId41" location="fourclass" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - fourclass" xr:uid="{F099ACB8-1D7C-4608-8C6F-337950DE428D}"/>
     <hyperlink ref="E2" r:id="rId42" location="TKH96a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - TKH96a" xr:uid="{E85386DD-0823-407B-BA91-BD8B86A47C4F}"/>
     <hyperlink ref="A35" r:id="rId43" location="german.numer" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - german.numer" xr:uid="{46E33753-7EFC-4CFB-B9E5-8B1C5C256128}"/>
     <hyperlink ref="E35" r:id="rId44" display="http://www.liacc.up.pt/ML/old/statlog/datasets.html" xr:uid="{B0BE7DBF-C3DB-4DD9-9D08-7D075B94B7A5}"/>
     <hyperlink ref="A83" r:id="rId45" location="gisette" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - gisette" xr:uid="{59B6FC79-9D71-43FB-A469-295CFB505BCB}"/>
-    <hyperlink ref="A22" r:id="rId46" location="heart" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - heart" xr:uid="{F9251AE3-2D08-414F-9980-61AEA66D16DB}"/>
-    <hyperlink ref="E22" r:id="rId47" display="http://www.liacc.up.pt/ML/old/statlog/datasets.html" xr:uid="{53362938-B035-4750-9128-BDA7C91A5971}"/>
+    <hyperlink ref="A21" r:id="rId46" location="heart" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - heart" xr:uid="{F9251AE3-2D08-414F-9980-61AEA66D16DB}"/>
+    <hyperlink ref="E21" r:id="rId47" display="http://www.liacc.up.pt/ML/old/statlog/datasets.html" xr:uid="{53362938-B035-4750-9128-BDA7C91A5971}"/>
     <hyperlink ref="A37" r:id="rId48" location="HIGGS" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - HIGGS" xr:uid="{6B14FB05-594E-40DA-A311-37A4218C0189}"/>
     <hyperlink ref="E37" r:id="rId49" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{94185930-FDC0-44F0-BA8F-A5355F04D816}"/>
     <hyperlink ref="A34" r:id="rId50" location="ijcnn1" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - ijcnn1" xr:uid="{0DBB04E9-DEA4-4F1D-9558-297730AF1D25}"/>
@@ -3385,69 +3385,69 @@
     <hyperlink ref="E101" r:id="rId70" location="SSK05a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - SSK05a" xr:uid="{200E2D20-4BB9-42BA-94A4-85BBD7A30220}"/>
     <hyperlink ref="A48" r:id="rId71" location="phishing" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - phishing" xr:uid="{1526BB69-4152-495E-8952-555B3DC4B1BD}"/>
     <hyperlink ref="E48" r:id="rId72" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{AAE1CBE4-4009-449A-ACDE-6460061393B1}"/>
-    <hyperlink ref="A91" r:id="rId73" location="rcv1.binary" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - rcv1.binary" xr:uid="{937E9592-10D0-4FCB-8318-AD1EA781F15C}"/>
-    <hyperlink ref="E91" r:id="rId74" location="DL04b" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - DL04b" xr:uid="{1CF58B97-5D97-4C7E-BF85-B4425222C8FC}"/>
+    <hyperlink ref="A88" r:id="rId73" location="rcv1.binary" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - rcv1.binary" xr:uid="{937E9592-10D0-4FCB-8318-AD1EA781F15C}"/>
+    <hyperlink ref="E88" r:id="rId74" location="DL04b" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - DL04b" xr:uid="{1CF58B97-5D97-4C7E-BF85-B4425222C8FC}"/>
     <hyperlink ref="A86" r:id="rId75" location="real-sim" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - real-sim" xr:uid="{FE72D1BD-999D-4CC5-8CAB-B4A2BD3740C4}"/>
     <hyperlink ref="E86" r:id="rId76" display="http://www.cs.umass.edu/~mccallum/code-data.html" xr:uid="{5A1081A0-5A48-40F0-A26E-8FF1247F630F}"/>
     <hyperlink ref="A3" r:id="rId77" location="skin_nonskin" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - skin_nonskin" xr:uid="{E98D364C-90D9-4543-BBC8-4707A94F7349}"/>
     <hyperlink ref="E3" r:id="rId78" display="https://archive.ics.uci.edu/ml/datasets/Skin+Segmentation" xr:uid="{3E60A4A1-BF76-43BF-A60E-DCAC1EE7F1C4}"/>
-    <hyperlink ref="A45" r:id="rId79" location="splice" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - splice" xr:uid="{DA08D226-FE85-41A4-88FB-AD14D2F9E958}"/>
-    <hyperlink ref="E45" r:id="rId80" display="http://www.cs.toronto.edu/~delve/data/datasets.html" xr:uid="{7DE2ACE8-C108-4C90-A085-ED56A17285F1}"/>
+    <hyperlink ref="A46" r:id="rId79" location="splice" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - splice" xr:uid="{DA08D226-FE85-41A4-88FB-AD14D2F9E958}"/>
+    <hyperlink ref="E46" r:id="rId80" display="http://www.cs.toronto.edu/~delve/data/datasets.html" xr:uid="{7DE2ACE8-C108-4C90-A085-ED56A17285F1}"/>
     <hyperlink ref="A104" r:id="rId81" location="splice-site" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - splice-site" xr:uid="{B9DFBE2D-1511-43E5-87B2-307445D221A6}"/>
     <hyperlink ref="E104" r:id="rId82" location="SS10a,AA12a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - SS10a,AA12a" xr:uid="{90E2BFAA-FB7D-44D0-BAC1-7F2D64C5B144}"/>
-    <hyperlink ref="A46" r:id="rId83" location="sonar" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - sonar" xr:uid="{7853A5DB-3933-4A9C-BCFA-F199F01E0F68}"/>
-    <hyperlink ref="E46" r:id="rId84" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{3132EE03-9621-4731-80FB-6458140401B1}"/>
+    <hyperlink ref="A45" r:id="rId83" location="sonar" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - sonar" xr:uid="{7853A5DB-3933-4A9C-BCFA-F199F01E0F68}"/>
+    <hyperlink ref="E45" r:id="rId84" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{3132EE03-9621-4731-80FB-6458140401B1}"/>
     <hyperlink ref="A29" r:id="rId85" location="SUSY" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - SUSY" xr:uid="{CF818986-B7FC-46FB-B0FD-C5EEEBED433D}"/>
     <hyperlink ref="E29" r:id="rId86" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{7BA8AB74-ECDB-4E04-A7C9-B30B61929976}"/>
-    <hyperlink ref="A4" r:id="rId87" location="svmguide1" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - svmguide1" xr:uid="{6BEE6DD3-6258-46C0-95ED-4154B1EB3BAE}"/>
-    <hyperlink ref="E4" r:id="rId88" location="CWH03a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - CWH03a" xr:uid="{B0EEA58A-AA76-4767-8F1E-E101AEFFF453}"/>
+    <hyperlink ref="A5" r:id="rId87" location="svmguide1" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - svmguide1" xr:uid="{6BEE6DD3-6258-46C0-95ED-4154B1EB3BAE}"/>
+    <hyperlink ref="E5" r:id="rId88" location="CWH03a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - CWH03a" xr:uid="{B0EEA58A-AA76-4767-8F1E-E101AEFFF453}"/>
     <hyperlink ref="A33" r:id="rId89" location="svmguide3" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - svmguide3" xr:uid="{24FDA6F3-B160-4302-93AD-A8D14F5921AE}"/>
     <hyperlink ref="E33" r:id="rId90" location="CWH03a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - CWH03a" xr:uid="{3201B2FF-6E1C-4C84-8199-FCC3E2FB1A8E}"/>
     <hyperlink ref="A102" r:id="rId91" location="url" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - url" xr:uid="{FF1D16A1-2854-4025-A3A4-9C1C77B84CBE}"/>
     <hyperlink ref="E102" r:id="rId92" location="JM09a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - JM09a" xr:uid="{2A6164B9-BFF6-4D67-A5F4-7F7987118696}"/>
-    <hyperlink ref="A75" r:id="rId93" location="w1a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - w1a" xr:uid="{92569D94-E2BC-46E0-BDF9-A133932D621E}"/>
-    <hyperlink ref="E75" r:id="rId94" location="JP98a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - JP98a" xr:uid="{AF8508D6-D9C9-484F-BB61-3AFCB4535EB2}"/>
-    <hyperlink ref="A74" r:id="rId95" location="w2a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - w2a" xr:uid="{3DB30826-D053-41FB-9F1B-2B2205396072}"/>
-    <hyperlink ref="E74" r:id="rId96" location="JP98a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - JP98a" xr:uid="{5BB2AEB1-B96E-4085-A59E-2C25EE4723C6}"/>
-    <hyperlink ref="A73" r:id="rId97" location="w3a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - w3a" xr:uid="{8839C821-9CF8-4FF9-B94A-38503AD0039A}"/>
-    <hyperlink ref="E73" r:id="rId98" location="JP98a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - JP98a" xr:uid="{234B7530-D7AF-4BFE-81B2-1AD2E8B8AEEA}"/>
-    <hyperlink ref="A72" r:id="rId99" location="w4a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - w4a" xr:uid="{BFF6CE5E-8EAC-4A97-9594-19D0FF2697F6}"/>
-    <hyperlink ref="E72" r:id="rId100" location="JP98a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - JP98a" xr:uid="{127AD052-61AC-4587-AE32-B20F366284B1}"/>
-    <hyperlink ref="A71" r:id="rId101" location="w5a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - w5a" xr:uid="{7F5491BD-AE0A-4BDD-8697-D06E95F37552}"/>
-    <hyperlink ref="E71" r:id="rId102" location="JP98a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - JP98a" xr:uid="{9E20086D-929C-4BF1-A15A-45FF83ECD16C}"/>
-    <hyperlink ref="A70" r:id="rId103" location="w6a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - w6a" xr:uid="{EB45F3EB-117C-4151-876D-D05C5CF7D69D}"/>
-    <hyperlink ref="E70" r:id="rId104" location="JP98a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - JP98a" xr:uid="{D40279B2-D7B1-48E9-9140-9CD4EC037076}"/>
-    <hyperlink ref="A69" r:id="rId105" location="w7a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - w7a" xr:uid="{F8927125-D883-4CDF-BCA1-ADD2BD9FBBD5}"/>
-    <hyperlink ref="E69" r:id="rId106" location="JP98a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - JP98a" xr:uid="{0BA40F3E-31D4-49C3-BB4D-40558199DBD3}"/>
-    <hyperlink ref="A68" r:id="rId107" location="w8a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - w8a" xr:uid="{0B2A46DB-F346-4C48-AD28-6D90F2D13CAD}"/>
-    <hyperlink ref="E68" r:id="rId108" location="JP98a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - JP98a" xr:uid="{13B0F123-091E-4045-BC19-28718868A7D3}"/>
+    <hyperlink ref="A68" r:id="rId93" location="w1a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - w1a" xr:uid="{92569D94-E2BC-46E0-BDF9-A133932D621E}"/>
+    <hyperlink ref="E68" r:id="rId94" location="JP98a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - JP98a" xr:uid="{AF8508D6-D9C9-484F-BB61-3AFCB4535EB2}"/>
+    <hyperlink ref="A69" r:id="rId95" location="w2a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - w2a" xr:uid="{3DB30826-D053-41FB-9F1B-2B2205396072}"/>
+    <hyperlink ref="E69" r:id="rId96" location="JP98a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - JP98a" xr:uid="{5BB2AEB1-B96E-4085-A59E-2C25EE4723C6}"/>
+    <hyperlink ref="A70" r:id="rId97" location="w3a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - w3a" xr:uid="{8839C821-9CF8-4FF9-B94A-38503AD0039A}"/>
+    <hyperlink ref="E70" r:id="rId98" location="JP98a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - JP98a" xr:uid="{234B7530-D7AF-4BFE-81B2-1AD2E8B8AEEA}"/>
+    <hyperlink ref="A71" r:id="rId99" location="w4a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - w4a" xr:uid="{BFF6CE5E-8EAC-4A97-9594-19D0FF2697F6}"/>
+    <hyperlink ref="E71" r:id="rId100" location="JP98a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - JP98a" xr:uid="{127AD052-61AC-4587-AE32-B20F366284B1}"/>
+    <hyperlink ref="A72" r:id="rId101" location="w5a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - w5a" xr:uid="{7F5491BD-AE0A-4BDD-8697-D06E95F37552}"/>
+    <hyperlink ref="E72" r:id="rId102" location="JP98a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - JP98a" xr:uid="{9E20086D-929C-4BF1-A15A-45FF83ECD16C}"/>
+    <hyperlink ref="A73" r:id="rId103" location="w6a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - w6a" xr:uid="{EB45F3EB-117C-4151-876D-D05C5CF7D69D}"/>
+    <hyperlink ref="E73" r:id="rId104" location="JP98a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - JP98a" xr:uid="{D40279B2-D7B1-48E9-9140-9CD4EC037076}"/>
+    <hyperlink ref="A74" r:id="rId105" location="w7a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - w7a" xr:uid="{F8927125-D883-4CDF-BCA1-ADD2BD9FBBD5}"/>
+    <hyperlink ref="E74" r:id="rId106" location="JP98a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - JP98a" xr:uid="{0BA40F3E-31D4-49C3-BB4D-40558199DBD3}"/>
+    <hyperlink ref="A75" r:id="rId107" location="w8a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - w8a" xr:uid="{0B2A46DB-F346-4C48-AD28-6D90F2D13CAD}"/>
+    <hyperlink ref="E75" r:id="rId108" location="JP98a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - JP98a" xr:uid="{13B0F123-091E-4045-BC19-28718868A7D3}"/>
     <hyperlink ref="A105" r:id="rId109" location="webspam" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/binary.html - webspam" xr:uid="{5B5A8851-DD63-4FFF-B85F-1BD049AC9452}"/>
     <hyperlink ref="A64" r:id="rId110" location="aloi" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - aloi" xr:uid="{09DC1B9A-985A-4BE7-844C-4AE00605BAEA}"/>
     <hyperlink ref="A63" r:id="rId111" location="connect-4" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - connect-4" xr:uid="{5C13F77F-ED83-485F-80E3-1E6270108905}"/>
     <hyperlink ref="E63" r:id="rId112" display="http://archive.ics.uci.edu/ml/machine-learning-databases/connect-4/" xr:uid="{C387D61D-8D21-4EE2-888E-F662C04EB6A3}"/>
-    <hyperlink ref="A44" r:id="rId113" location="covtype" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - covtype" xr:uid="{8A9F3E31-B221-4867-9845-7B0318B73DAE}"/>
-    <hyperlink ref="E44" r:id="rId114" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{282A4870-C035-4443-A511-66EC6DABC7F2}"/>
+    <hyperlink ref="A43" r:id="rId113" location="covtype" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - covtype" xr:uid="{8A9F3E31-B221-4867-9845-7B0318B73DAE}"/>
+    <hyperlink ref="E43" r:id="rId114" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{282A4870-C035-4443-A511-66EC6DABC7F2}"/>
     <hyperlink ref="A65" r:id="rId115" location="dna" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - dna" xr:uid="{EE0BAB1F-AB93-47D6-B68E-420E70BBCA01}"/>
     <hyperlink ref="E65" r:id="rId116" display="http://www.liacc.up.pt/ML/old/statlog/datasets.html" xr:uid="{47369B12-5D86-4BF7-A1BA-160E6ACCF1BD}"/>
-    <hyperlink ref="A15" r:id="rId117" location="glass" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - glass" xr:uid="{509852D4-3EA2-4147-9D85-A045207A86EF}"/>
-    <hyperlink ref="E15" r:id="rId118" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{9491FE34-A346-418B-A3E1-84268724246C}"/>
-    <hyperlink ref="A5" r:id="rId119" location="iris" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - iris" xr:uid="{2901399E-47D5-488E-8B0E-87666B4BA2CE}"/>
-    <hyperlink ref="E5" r:id="rId120" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{853CCD2D-2F88-4B08-A9A2-98D5C867C144}"/>
-    <hyperlink ref="A26" r:id="rId121" location="letter" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - letter" xr:uid="{6D69B477-226B-46F1-9930-532CEDDE90D5}"/>
-    <hyperlink ref="E26" r:id="rId122" display="http://www.liacc.up.pt/ML/old/statlog/datasets.html" xr:uid="{049DE2E4-3FF5-42F4-8592-66DC10116606}"/>
+    <hyperlink ref="A14" r:id="rId117" location="glass" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - glass" xr:uid="{509852D4-3EA2-4147-9D85-A045207A86EF}"/>
+    <hyperlink ref="E14" r:id="rId118" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{9491FE34-A346-418B-A3E1-84268724246C}"/>
+    <hyperlink ref="A4" r:id="rId119" location="iris" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - iris" xr:uid="{2901399E-47D5-488E-8B0E-87666B4BA2CE}"/>
+    <hyperlink ref="E4" r:id="rId120" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{853CCD2D-2F88-4B08-A9A2-98D5C867C144}"/>
+    <hyperlink ref="A27" r:id="rId121" location="letter" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - letter" xr:uid="{6D69B477-226B-46F1-9930-532CEDDE90D5}"/>
+    <hyperlink ref="E27" r:id="rId122" display="http://www.liacc.up.pt/ML/old/statlog/datasets.html" xr:uid="{049DE2E4-3FF5-42F4-8592-66DC10116606}"/>
     <hyperlink ref="A78" r:id="rId123" location="mnist" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - mnist" xr:uid="{B3385105-1426-45B7-982D-8400D6D85A4C}"/>
     <hyperlink ref="E78" r:id="rId124" location="YL98a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - YL98a" xr:uid="{FC97FA92-8F5D-4990-8F13-19277FFE8100}"/>
     <hyperlink ref="A79" r:id="rId125" location="mnist8m" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - mnist8m" xr:uid="{09181B0E-18DA-4AB1-80A6-1350CB820F30}"/>
     <hyperlink ref="A95" r:id="rId126" location="news20" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - news20" xr:uid="{F4453691-E5F8-40B6-9658-7B45DBBB6400}"/>
     <hyperlink ref="E95" r:id="rId127" location="KL95a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - KL95a" xr:uid="{58F53F3C-805B-4F0C-A92F-EFE885A3B080}"/>
-    <hyperlink ref="A27" r:id="rId128" location="pendigits" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - pendigits" xr:uid="{0B652887-D08D-43A8-AAEB-844BF6F3F64B}"/>
-    <hyperlink ref="E27" r:id="rId129" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{7D47967F-767E-4602-975D-327B4A32ACC2}"/>
-    <hyperlink ref="A16" r:id="rId130" location="poker" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - poker" xr:uid="{25D11298-DBE0-4A36-BD0F-EF921DC0E3B7}"/>
-    <hyperlink ref="E16" r:id="rId131" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{5C5AF6F5-804C-4D9F-A971-C6441FDEB4B1}"/>
+    <hyperlink ref="A28" r:id="rId128" location="pendigits" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - pendigits" xr:uid="{0B652887-D08D-43A8-AAEB-844BF6F3F64B}"/>
+    <hyperlink ref="E28" r:id="rId129" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{7D47967F-767E-4602-975D-327B4A32ACC2}"/>
+    <hyperlink ref="A17" r:id="rId130" location="poker" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - poker" xr:uid="{25D11298-DBE0-4A36-BD0F-EF921DC0E3B7}"/>
+    <hyperlink ref="E17" r:id="rId131" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{5C5AF6F5-804C-4D9F-A971-C6441FDEB4B1}"/>
     <hyperlink ref="A76" r:id="rId132" location="protein" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - protein" xr:uid="{A6D869FB-46C3-44B0-95C3-B0B49BC69346}"/>
     <hyperlink ref="E76" r:id="rId133" location="JYW02a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - JYW02a" xr:uid="{63DCC4E8-98F9-435A-8DC1-DC0538233DDA}"/>
-    <hyperlink ref="A92" r:id="rId134" location="rcv1.multiclass" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - rcv1.multiclass" xr:uid="{036333AC-85CC-474A-8E6C-A532A65BF0E7}"/>
-    <hyperlink ref="E92" r:id="rId135" location="DL04b" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - DL04b" xr:uid="{EBEFB677-95CF-4E62-8CB5-B9C8F2E9199D}"/>
+    <hyperlink ref="A89" r:id="rId134" location="rcv1.multiclass" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - rcv1.multiclass" xr:uid="{036333AC-85CC-474A-8E6C-A532A65BF0E7}"/>
+    <hyperlink ref="E89" r:id="rId135" location="DL04b" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - DL04b" xr:uid="{EBEFB677-95CF-4E62-8CB5-B9C8F2E9199D}"/>
     <hyperlink ref="A39" r:id="rId136" location="satimage" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - satimage" xr:uid="{D194C6EB-A2C5-404D-8D15-E8D5A24D0F99}"/>
     <hyperlink ref="E39" r:id="rId137" display="http://www.liacc.up.pt/ML/old/statlog/datasets.html" xr:uid="{804AFF17-AED7-448E-8C9A-BC0F7841D0CD}"/>
     <hyperlink ref="A94" r:id="rId138" location="sector" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - sector" xr:uid="{EE1DF62F-3F1A-4906-8A11-A01D69D5CE39}"/>
@@ -3456,13 +3456,13 @@
     <hyperlink ref="E31" r:id="rId141" display="http://www.liacc.up.pt/ML/old/statlog/datasets.html" xr:uid="{939646D0-6BA0-4BE1-96E0-0DDE246DC16C}"/>
     <hyperlink ref="A40" r:id="rId142" location="Sensorless" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - Sensorless" xr:uid="{AE493A47-C385-4CFE-AC2B-C6EE61D6C790}"/>
     <hyperlink ref="E40" r:id="rId143" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{CF459F5E-E444-4B45-95CE-9F8082B23045}"/>
-    <hyperlink ref="A14" r:id="rId144" location="shuttle" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - shuttle" xr:uid="{D39AC275-4084-4D9D-AB06-1F9F6CD0A30B}"/>
-    <hyperlink ref="E14" r:id="rId145" display="http://www.liacc.up.pt/ML/old/statlog/datasets.html" xr:uid="{8F7F2FA9-0283-465B-9ECA-6D1DE01F5929}"/>
+    <hyperlink ref="A15" r:id="rId144" location="shuttle" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - shuttle" xr:uid="{D39AC275-4084-4D9D-AB06-1F9F6CD0A30B}"/>
+    <hyperlink ref="E15" r:id="rId145" display="http://www.liacc.up.pt/ML/old/statlog/datasets.html" xr:uid="{8F7F2FA9-0283-465B-9ECA-6D1DE01F5929}"/>
     <hyperlink ref="A82" r:id="rId146" location="SVHN" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - SVHN" xr:uid="{44E19F31-663A-456F-BD90-2E8A6FA99147}"/>
     <hyperlink ref="A32" r:id="rId147" location="svmguide2" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - svmguide2" xr:uid="{44EEF749-B733-4A66-B354-96BCEC7BF938}"/>
     <hyperlink ref="E32" r:id="rId148" location="CWH03a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - CWH03a" xr:uid="{5BC57EC5-3234-45B5-8308-A1BF8ACBB4D2}"/>
-    <hyperlink ref="A19" r:id="rId149" location="svmguide4" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - svmguide4" xr:uid="{EEC916FD-3388-4F91-B1CD-682B6485D8E9}"/>
-    <hyperlink ref="E19" r:id="rId150" location="CWH03a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - CWH03a" xr:uid="{849E28BA-1595-45A4-A7CB-E56E241339D2}"/>
+    <hyperlink ref="A18" r:id="rId149" location="svmguide4" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - svmguide4" xr:uid="{EEC916FD-3388-4F91-B1CD-682B6485D8E9}"/>
+    <hyperlink ref="E18" r:id="rId150" location="CWH03a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - CWH03a" xr:uid="{849E28BA-1595-45A4-A7CB-E56E241339D2}"/>
     <hyperlink ref="A66" r:id="rId151" location="usps" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - usps" xr:uid="{120E2BE7-2913-4C25-8424-C54CA43443F8}"/>
     <hyperlink ref="E66" r:id="rId152" location="JJH94a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - JJH94a" xr:uid="{D9853E84-060F-4044-A606-76CF44698B6C}"/>
     <hyperlink ref="A41" r:id="rId153" location="SensIT%20Vehicle%20(acoustic)" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - SensIT%20Vehicle%20(acoustic)" xr:uid="{5B337C98-9754-4371-8D10-B42C1EDA1A94}"/>
@@ -3470,12 +3470,12 @@
     <hyperlink ref="A50" r:id="rId155" location="SensIT%20Vehicle%20(combined)" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - SensIT%20Vehicle%20(combined)" xr:uid="{772BE455-E75E-4DBA-915C-B427CA7B8654}"/>
     <hyperlink ref="A30" r:id="rId156" location="vehicle" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - vehicle" xr:uid="{91A0A04F-3282-455D-8E8E-E0136413D1C1}"/>
     <hyperlink ref="E30" r:id="rId157" display="http://www.liacc.up.pt/ML/old/statlog/datasets.html" xr:uid="{6A731DE3-7475-4495-A32C-665942BA1647}"/>
-    <hyperlink ref="A18" r:id="rId158" location="vowel" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - vowel" xr:uid="{E8509E76-E927-42CA-9F71-78C09576D7F3}"/>
-    <hyperlink ref="E18" r:id="rId159" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{9C29889E-9E44-4064-9BD4-396E6E190233}"/>
+    <hyperlink ref="A19" r:id="rId158" location="vowel" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - vowel" xr:uid="{E8509E76-E927-42CA-9F71-78C09576D7F3}"/>
+    <hyperlink ref="E19" r:id="rId159" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{9C29889E-9E44-4064-9BD4-396E6E190233}"/>
     <hyperlink ref="A23" r:id="rId160" location="wine" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multiclass.html - wine" xr:uid="{4E1BAEF7-085E-43C1-A1F0-71A69F71F6A7}"/>
     <hyperlink ref="E23" r:id="rId161" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{0958FCDC-27A8-4C8B-A32F-8B35CCA0630F}"/>
-    <hyperlink ref="A12" r:id="rId162" location="abalone" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/regression.html - abalone" xr:uid="{0F0CAD9B-DC7A-4B1D-9886-D195BCED2D99}"/>
-    <hyperlink ref="E12" r:id="rId163" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{A91C88F2-7665-4967-A668-5507C50B3A82}"/>
+    <hyperlink ref="A10" r:id="rId162" location="abalone" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/regression.html - abalone" xr:uid="{0F0CAD9B-DC7A-4B1D-9886-D195BCED2D99}"/>
+    <hyperlink ref="E10" r:id="rId163" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{A91C88F2-7665-4967-A668-5507C50B3A82}"/>
     <hyperlink ref="A25" r:id="rId164" location="bodyfat" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/regression.html - bodyfat" xr:uid="{683B8AA2-288B-463B-A3C9-D867FAE09CD7}"/>
     <hyperlink ref="E25" r:id="rId165" display="http://lib.stat.cmu.edu/datasets/" xr:uid="{2D2F0C84-3138-460B-B4C5-FEEB99A1B46A}"/>
     <hyperlink ref="A11" r:id="rId166" location="cadata" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/regression.html - cadata" xr:uid="{2E645219-58DD-48AE-9C74-BB99CB157EAD}"/>
@@ -3486,17 +3486,17 @@
     <hyperlink ref="E103" r:id="rId171" display="http://www.ark.cs.cmu.edu/10K/" xr:uid="{750E361C-B1EF-4ED4-84A2-76BD0094BCAA}"/>
     <hyperlink ref="A96" r:id="rId172" location="E2006-tfidf" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/regression.html - E2006-tfidf" xr:uid="{1D637DAF-CC6F-4CFD-BE66-8F6455152FEE}"/>
     <hyperlink ref="E96" r:id="rId173" display="http://www.ark.cs.cmu.edu/10K/" xr:uid="{B060FBDA-BBD9-49A5-942E-B7B045E06DD6}"/>
-    <hyperlink ref="A28" r:id="rId174" location="eunite2001" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/regression.html - eunite2001" xr:uid="{A39EF022-E1CB-4AF7-9CE2-F721797AAC53}"/>
-    <hyperlink ref="A21" r:id="rId175" location="housing" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/regression.html - housing" xr:uid="{94C1D6D3-7251-4FA0-8795-F97EA925FF81}"/>
-    <hyperlink ref="E21" r:id="rId176" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{C28406D7-DE93-4D0D-A050-BE81E90B4466}"/>
-    <hyperlink ref="A8" r:id="rId177" location="mg" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/regression.html - mg" xr:uid="{764017F1-167A-4FEE-BB90-C72B30CAC0DB}"/>
-    <hyperlink ref="E8" r:id="rId178" location="GWF01a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - GWF01a" xr:uid="{763B128D-6C27-463A-8070-B938C831F99F}"/>
+    <hyperlink ref="A26" r:id="rId174" location="eunite2001" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/regression.html - eunite2001" xr:uid="{A39EF022-E1CB-4AF7-9CE2-F721797AAC53}"/>
+    <hyperlink ref="A22" r:id="rId175" location="housing" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/regression.html - housing" xr:uid="{94C1D6D3-7251-4FA0-8795-F97EA925FF81}"/>
+    <hyperlink ref="E22" r:id="rId176" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{C28406D7-DE93-4D0D-A050-BE81E90B4466}"/>
+    <hyperlink ref="A7" r:id="rId177" location="mg" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/regression.html - mg" xr:uid="{764017F1-167A-4FEE-BB90-C72B30CAC0DB}"/>
+    <hyperlink ref="E7" r:id="rId178" location="GWF01a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - GWF01a" xr:uid="{763B128D-6C27-463A-8070-B938C831F99F}"/>
     <hyperlink ref="A9" r:id="rId179" location="mpg" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/regression.html - mpg" xr:uid="{24E0D20E-FDD6-43D3-B09F-F8FD5757A902}"/>
     <hyperlink ref="E9" r:id="rId180" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{A8D0CD42-553A-42C5-AFBA-6B34AF1801C6}"/>
     <hyperlink ref="A36" r:id="rId181" location="pyrim" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/regression.html - pyrim" xr:uid="{42BD66E3-4AA3-4C99-80E7-744AA38AA9E3}"/>
     <hyperlink ref="E36" r:id="rId182" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{2B4F0A4F-6C9A-4BB7-8343-EF63DE7079BC}"/>
-    <hyperlink ref="A7" r:id="rId183" location="space_ga" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/regression.html - space_ga" xr:uid="{C912586D-A5EB-4D37-A40A-54E633FD012D}"/>
-    <hyperlink ref="E7" r:id="rId184" display="http://lib.stat.cmu.edu/datasets/" xr:uid="{5476A6EF-C6F9-475D-BBEE-CDC8AEA7A2FB}"/>
+    <hyperlink ref="A8" r:id="rId183" location="space_ga" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/regression.html - space_ga" xr:uid="{C912586D-A5EB-4D37-A40A-54E633FD012D}"/>
+    <hyperlink ref="E8" r:id="rId184" display="http://lib.stat.cmu.edu/datasets/" xr:uid="{5476A6EF-C6F9-475D-BBEE-CDC8AEA7A2FB}"/>
     <hyperlink ref="A47" r:id="rId185" location="triazines" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/regression.html - triazines" xr:uid="{397C1821-BE11-4C52-A902-9803634912A3}"/>
     <hyperlink ref="E47" r:id="rId186" display="http://www.ics.uci.edu/~mlearn/MLRepository.html" xr:uid="{F6FDA19E-02CF-41BC-8D74-38BABEA80D4E}"/>
     <hyperlink ref="A49" r:id="rId187" location="YearPredictionMSD" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/regression.html - YearPredictionMSD" xr:uid="{6696EC93-82FB-405E-A69C-3D6EFCA5243C}"/>
@@ -3505,12 +3505,12 @@
     <hyperlink ref="E53" r:id="rId190" display="http://www.mediamill.nl/challenge/" xr:uid="{C21EABAB-CA9C-45D7-A837-842101385AAA}"/>
     <hyperlink ref="A93" r:id="rId191" location="rcv1v2%20(topics;%20subsets)" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multilabel.html - rcv1v2%20(topics;%20subsets)" xr:uid="{50EBEFF6-166F-474F-A0A0-0E1C768BCC56}"/>
     <hyperlink ref="E93" r:id="rId192" location="DL04b" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - DL04b" xr:uid="{663B286C-D3D0-42DC-98D3-E113864E475A}"/>
-    <hyperlink ref="A88" r:id="rId193" location="rcv1v2%20(topics;%20full%20sets)" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multilabel.html - rcv1v2%20(topics;%20full%20sets)" xr:uid="{D854D945-52E5-47D7-8E39-7A9FD7C7A468}"/>
-    <hyperlink ref="E88" r:id="rId194" location="DL04b" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - DL04b" xr:uid="{65E5034A-3A56-47A2-8703-E300771356DB}"/>
-    <hyperlink ref="A89" r:id="rId195" location="rcv1v2%20(industries;%20full%20sets)" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multilabel.html - rcv1v2%20(industries;%20full%20sets)" xr:uid="{49FCE16C-F30B-4774-A3E5-D92B638626D2}"/>
-    <hyperlink ref="E89" r:id="rId196" location="DL04b" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - DL04b" xr:uid="{77C25E9F-9409-491B-8E46-7C59E3021387}"/>
-    <hyperlink ref="A90" r:id="rId197" location="rcv1v2%20(regions;%20full%20sets)" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multilabel.html - rcv1v2%20(regions;%20full%20sets)" xr:uid="{A8DFC2BB-2FAF-47F3-99A2-F67C0BE8A82C}"/>
-    <hyperlink ref="E90" r:id="rId198" location="DL04b" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - DL04b" xr:uid="{EB2D87AA-1B8A-4B9C-B944-653D1E27881A}"/>
+    <hyperlink ref="A92" r:id="rId193" location="rcv1v2%20(topics;%20full%20sets)" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multilabel.html - rcv1v2%20(topics;%20full%20sets)" xr:uid="{D854D945-52E5-47D7-8E39-7A9FD7C7A468}"/>
+    <hyperlink ref="E92" r:id="rId194" location="DL04b" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - DL04b" xr:uid="{65E5034A-3A56-47A2-8703-E300771356DB}"/>
+    <hyperlink ref="A90" r:id="rId195" location="rcv1v2%20(industries;%20full%20sets)" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multilabel.html - rcv1v2%20(industries;%20full%20sets)" xr:uid="{49FCE16C-F30B-4774-A3E5-D92B638626D2}"/>
+    <hyperlink ref="E90" r:id="rId196" location="DL04b" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - DL04b" xr:uid="{77C25E9F-9409-491B-8E46-7C59E3021387}"/>
+    <hyperlink ref="A91" r:id="rId197" location="rcv1v2%20(regions;%20full%20sets)" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multilabel.html - rcv1v2%20(regions;%20full%20sets)" xr:uid="{A8DFC2BB-2FAF-47F3-99A2-F67C0BE8A82C}"/>
+    <hyperlink ref="E91" r:id="rId198" location="DL04b" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - DL04b" xr:uid="{EB2D87AA-1B8A-4B9C-B944-653D1E27881A}"/>
     <hyperlink ref="A67" r:id="rId199" location="scene-classification" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multilabel.html - scene-classification" xr:uid="{28203FFF-F1F1-47B3-90BD-F67182E97115}"/>
     <hyperlink ref="E67" r:id="rId200" location="MB04a" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/ref.html - MB04a" xr:uid="{14756645-2EC2-4210-A141-331B539B8046}"/>
     <hyperlink ref="A87" r:id="rId201" location="siam-competition2007" display="https://www.csie.ntu.edu.tw/~cjlin/libsvmtools/datasets/multilabel.html - siam-competition2007" xr:uid="{500AC9E9-1F39-416B-B378-10A698A714AA}"/>

</xml_diff>